<commit_message>
michel et al and maek et al extractions + files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /full variability /raw data /bernhardt2018/bernhardt2018.xlsx
+++ b/data extraction /extraction /full variability /raw data /bernhardt2018/bernhardt2018.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /full variability /raw data /bernhardt2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15AB9335-C42A-954A-99AF-97906ACEF208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AAB289-D2E5-EF4B-BE21-A190FF7200F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-17820" windowWidth="27240" windowHeight="9940" activeTab="1" xr2:uid="{8E33FDED-3B24-0045-98A4-00A8B562CEB5}"/>
+    <workbookView xWindow="29160" yWindow="-25420" windowWidth="24000" windowHeight="9940" xr2:uid="{8E33FDED-3B24-0045-98A4-00A8B562CEB5}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,9 +112,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EC5771-DC97-AB4D-95F9-8F3BC31E8426}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C66433-9FA4-F441-A634-5FC115C3DFDE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>